<commit_message>
I need take the first derivative, not second, how i think later
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Николай\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26A0628-5585-4FA7-96FE-D2BDCA465FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A6112DE8-EE82-47D6-9E9F-7856A31969B5}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -62,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,28 +399,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71312370-4559-459E-99F7-16E2FD9BF699}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -455,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>500</v>
       </c>
@@ -484,7 +478,7 @@
         <v>5516320000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>750</v>
       </c>
@@ -513,7 +507,7 @@
         <v>8490570000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1000</v>
       </c>
@@ -542,7 +536,7 @@
         <v>9520250000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1250</v>
       </c>
@@ -571,7 +565,7 @@
         <v>4641110000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1500</v>
       </c>
@@ -600,7 +594,7 @@
         <v>820700000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2000</v>
       </c>
@@ -629,7 +623,7 @@
         <v>460000000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2500</v>
       </c>
@@ -658,7 +652,7 @@
         <v>320800000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3000</v>
       </c>

</xml_diff>